<commit_message>
datafil exempel med dummy koordinater och ingen adressinfo
</commit_message>
<xml_diff>
--- a/data_example1.xlsx
+++ b/data_example1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ltuppsala-my.sharepoint.com/personal/scb010_lul_se/Documents/git_projects/kollektivtrafikbarometer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDrive\OneDrive - Region Uppsala\git_projects\kollektivtrafikbarometer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E4FA7E-E438-4279-A680-B2200D3377C9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B30B3BB-B1F2-47EC-8D3B-5D47D016A111}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12375" xr2:uid="{65EF8BB7-1C21-4D4E-AB5E-55A7D8D76675}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5566" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5482" uniqueCount="422">
   <si>
     <t>A1</t>
   </si>
@@ -1122,12 +1122,6 @@
     <t>Stadstrafik</t>
   </si>
   <si>
-    <t>Bålsta station, Bålsta, Sverige</t>
-  </si>
-  <si>
-    <t>746 33 Bålsta, Sverige</t>
-  </si>
-  <si>
     <t>SE; Sverige</t>
   </si>
   <si>
@@ -1155,9 +1149,6 @@
     <t>Regionaltrafik</t>
   </si>
   <si>
-    <t>Bärbyleden, 752 28 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>752 28</t>
   </si>
   <si>
@@ -1170,12 +1161,6 @@
     <t>Man</t>
   </si>
   <si>
-    <t>Polacksbacken, Lägerhyddsvägen 2, Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>Lägerhyddsvägen 2, 752 37 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>752 37</t>
   </si>
   <si>
@@ -1185,9 +1170,6 @@
     <t>1/11/2018</t>
   </si>
   <si>
-    <t>SIMTUNA-HÖGBY 4, 749 72 Fjärdhundra, Sverige</t>
-  </si>
-  <si>
     <t>749 72</t>
   </si>
   <si>
@@ -1197,9 +1179,6 @@
     <t>Enköping N</t>
   </si>
   <si>
-    <t>Fredholmsgatan 22, 721 36 Västerås, Sverige</t>
-  </si>
-  <si>
     <t>Västmanlands län</t>
   </si>
   <si>
@@ -1224,12 +1203,6 @@
     <t>Enköping</t>
   </si>
   <si>
-    <t>Verkstadsgatan, Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>Verkstadsgatan, 753 23 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>753 23</t>
   </si>
   <si>
@@ -1239,15 +1212,6 @@
     <t>Östhammar</t>
   </si>
   <si>
-    <t>Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>Studenternas IP, Ulleråkersvägen, Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>Ulleråkersvägen 6, 753 09 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>753 09</t>
   </si>
   <si>
@@ -1269,9 +1233,6 @@
     <t>UPPSALA</t>
   </si>
   <si>
-    <t>Dragarbrunnsgatan 50A</t>
-  </si>
-  <si>
     <t>1/22/2018</t>
   </si>
   <si>
@@ -1281,18 +1242,12 @@
     <t>Söderfors</t>
   </si>
   <si>
-    <t>Ramsta-lund Lugnet 22, 755 91 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>755 91</t>
   </si>
   <si>
     <t>Uppsala V</t>
   </si>
   <si>
-    <t>Kryssbo 205, 748 95 Örbyhus, Sverige</t>
-  </si>
-  <si>
     <t>Kryssbo</t>
   </si>
   <si>
@@ -1305,9 +1260,6 @@
     <t>1/18/2018</t>
   </si>
   <si>
-    <t>Luthagen, Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>Luthagen</t>
   </si>
   <si>
@@ -1320,40 +1272,19 @@
     <t>1/10/2018</t>
   </si>
   <si>
-    <t>IFU Arena, Råbyvägen, Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>Råbyvägen 77, 754 26 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>754 26</t>
   </si>
   <si>
     <t>Gränby</t>
   </si>
   <si>
-    <t>Fjalars gränd, 753 19 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>753 19</t>
   </si>
   <si>
-    <t>Uppsala universitet, Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>Uppsala, 752 36 Uppsala, Sverige</t>
-  </si>
-  <si>
     <t>752 36</t>
   </si>
   <si>
     <t>Kåbo</t>
-  </si>
-  <si>
-    <t>Uppsala C, Uppsala, Sverige</t>
-  </si>
-  <si>
-    <t>753 21 Uppsala, Sverige</t>
   </si>
   <si>
     <t>753 21</t>
@@ -1366,6 +1297,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1395,9 +1329,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1712,11 +1647,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1327363F-302D-4319-8128-184323BD1D7F}">
-  <dimension ref="A1:MR20"/>
+  <dimension ref="A1:MR24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="HW1" workbookViewId="0">
+      <selection activeCell="IF10" sqref="IF10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="79" max="79" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="87" max="88" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="91" max="92" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="237" max="238" width="11" bestFit="1" customWidth="1"/>
+    <col min="247" max="248" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:356" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4093,11 +4038,13 @@
       <c r="BZ3" t="s">
         <v>356</v>
       </c>
-      <c r="CA3">
-        <v>59.573758599999998</v>
-      </c>
-      <c r="CB3">
-        <v>17.478649099999998</v>
+      <c r="CA3" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.349977547202315</v>
+      </c>
+      <c r="CB3" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.021069980620481</v>
       </c>
       <c r="CC3" t="s">
         <v>356</v>
@@ -4117,17 +4064,21 @@
       <c r="CH3" t="s">
         <v>356</v>
       </c>
-      <c r="CI3">
-        <v>59.569248600000002</v>
-      </c>
-      <c r="CJ3">
-        <v>17.531016000000001</v>
-      </c>
-      <c r="CK3">
-        <v>59.573758599999998</v>
-      </c>
-      <c r="CL3">
-        <v>17.478649099999998</v>
+      <c r="CI3" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.885609409220777</v>
+      </c>
+      <c r="CJ3" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.218635036935119</v>
+      </c>
+      <c r="CK3" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.979657722739653</v>
+      </c>
+      <c r="CL3" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.638306171198174</v>
       </c>
       <c r="CM3" t="s">
         <v>356</v>
@@ -4561,47 +4512,45 @@
       <c r="HZ3" t="s">
         <v>356</v>
       </c>
-      <c r="IA3" t="s">
-        <v>365</v>
-      </c>
-      <c r="IB3" t="s">
-        <v>366</v>
-      </c>
-      <c r="IC3">
-        <v>59.569248600000002</v>
-      </c>
-      <c r="ID3">
-        <v>17.531016000000001</v>
+      <c r="IC3" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.470443208296928</v>
+      </c>
+      <c r="ID3" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.974524506541417</v>
       </c>
       <c r="IE3" t="s">
         <v>362</v>
       </c>
       <c r="IF3" t="s">
+        <v>365</v>
+      </c>
+      <c r="IG3" t="s">
+        <v>366</v>
+      </c>
+      <c r="IH3" t="s">
         <v>367</v>
       </c>
-      <c r="IG3" t="s">
+      <c r="II3" t="s">
         <v>368</v>
       </c>
-      <c r="IH3" t="s">
+      <c r="IJ3" t="s">
         <v>369</v>
       </c>
-      <c r="II3" t="s">
-        <v>370</v>
-      </c>
-      <c r="IJ3" t="s">
-        <v>371</v>
-      </c>
       <c r="IK3" t="s">
         <v>356</v>
       </c>
       <c r="IL3" t="s">
         <v>356</v>
       </c>
-      <c r="IM3">
-        <v>59.573758599999998</v>
-      </c>
-      <c r="IN3">
-        <v>17.478649099999998</v>
+      <c r="IM3" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.648190764167332</v>
+      </c>
+      <c r="IN3" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.278658533277081</v>
       </c>
       <c r="IO3" t="s">
         <v>356</v>
@@ -4859,7 +4808,7 @@
         <v>171006795</v>
       </c>
       <c r="LV3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="LW3">
         <v>5.9753539379999996</v>
@@ -4874,13 +4823,13 @@
         <v>16</v>
       </c>
       <c r="MA3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="MB3">
         <v>1</v>
       </c>
       <c r="MC3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="MD3">
         <v>305</v>
@@ -4901,7 +4850,7 @@
         <v>74641</v>
       </c>
       <c r="MJ3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="MK3">
         <v>0</v>
@@ -4916,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="MO3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP3">
         <v>1</v>
@@ -5163,11 +5112,13 @@
       <c r="BZ4" t="s">
         <v>356</v>
       </c>
-      <c r="CA4">
-        <v>59.8703717</v>
-      </c>
-      <c r="CB4">
-        <v>17.644936699999999</v>
+      <c r="CA4" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.144646886768342</v>
+      </c>
+      <c r="CB4" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.071049014537252</v>
       </c>
       <c r="CC4" t="s">
         <v>356</v>
@@ -5187,17 +5138,21 @@
       <c r="CH4" t="s">
         <v>356</v>
       </c>
-      <c r="CI4">
-        <v>59.868540199999998</v>
-      </c>
-      <c r="CJ4">
-        <v>17.596741900000001</v>
-      </c>
-      <c r="CK4">
-        <v>59.8703717</v>
-      </c>
-      <c r="CL4">
-        <v>17.644936699999999</v>
+      <c r="CI4" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.748176736254443</v>
+      </c>
+      <c r="CJ4" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.62932928067821</v>
+      </c>
+      <c r="CK4" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.169474676646928</v>
+      </c>
+      <c r="CL4" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.373114390931232</v>
       </c>
       <c r="CM4" t="s">
         <v>356</v>
@@ -5631,35 +5586,31 @@
       <c r="HZ4" t="s">
         <v>356</v>
       </c>
-      <c r="IA4" t="s">
-        <v>376</v>
-      </c>
-      <c r="IB4" t="s">
-        <v>376</v>
-      </c>
-      <c r="IC4">
-        <v>59.868540199999998</v>
-      </c>
-      <c r="ID4">
-        <v>17.596741900000001</v>
+      <c r="IC4" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.261529677817819</v>
+      </c>
+      <c r="ID4" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.794258500431994</v>
       </c>
       <c r="IE4" t="s">
         <v>362</v>
       </c>
       <c r="IF4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG4" t="s">
         <v>360</v>
       </c>
       <c r="IH4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="II4" t="s">
         <v>360</v>
       </c>
       <c r="IJ4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IK4" t="s">
         <v>356</v>
@@ -5667,11 +5618,13 @@
       <c r="IL4" t="s">
         <v>356</v>
       </c>
-      <c r="IM4">
-        <v>59.8703717</v>
-      </c>
-      <c r="IN4">
-        <v>17.644936699999999</v>
+      <c r="IM4" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.128068340381148</v>
+      </c>
+      <c r="IN4" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.600266591838093</v>
       </c>
       <c r="IO4" t="s">
         <v>356</v>
@@ -5929,7 +5882,7 @@
         <v>171020107</v>
       </c>
       <c r="LV4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="LW4">
         <v>5.3887722599999996</v>
@@ -6701,12 +6654,6 @@
       <c r="HZ5" t="s">
         <v>356</v>
       </c>
-      <c r="IA5" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB5" t="s">
-        <v>356</v>
-      </c>
       <c r="IC5" t="s">
         <v>356</v>
       </c>
@@ -6930,7 +6877,7 @@
         <v>4</v>
       </c>
       <c r="KY5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="KZ5">
         <v>0</v>
@@ -6999,7 +6946,7 @@
         <v>171200221</v>
       </c>
       <c r="LV5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="LW5" t="s">
         <v>356</v>
@@ -7026,7 +6973,7 @@
         <v>380</v>
       </c>
       <c r="ME5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF5">
         <v>1</v>
@@ -7303,11 +7250,13 @@
       <c r="BZ6" t="s">
         <v>356</v>
       </c>
-      <c r="CA6">
-        <v>59.859152799999997</v>
-      </c>
-      <c r="CB6">
-        <v>17.6563135</v>
+      <c r="CA6" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.512274379105918</v>
+      </c>
+      <c r="CB6" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.008340533855396</v>
       </c>
       <c r="CC6" t="s">
         <v>356</v>
@@ -7327,17 +7276,21 @@
       <c r="CH6" t="s">
         <v>356</v>
       </c>
-      <c r="CI6">
-        <v>59.840981900000003</v>
-      </c>
-      <c r="CJ6">
-        <v>17.649445199999999</v>
-      </c>
-      <c r="CK6">
-        <v>59.859152799999997</v>
-      </c>
-      <c r="CL6">
-        <v>17.6563135</v>
+      <c r="CI6" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.28530916035438</v>
+      </c>
+      <c r="CJ6" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.892394517389327</v>
+      </c>
+      <c r="CK6" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.401974726367499</v>
+      </c>
+      <c r="CL6" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.217760260903347</v>
       </c>
       <c r="CM6" t="s">
         <v>356</v>
@@ -7771,35 +7724,31 @@
       <c r="HZ6" t="s">
         <v>356</v>
       </c>
-      <c r="IA6" t="s">
-        <v>381</v>
-      </c>
-      <c r="IB6" t="s">
-        <v>382</v>
-      </c>
-      <c r="IC6">
-        <v>59.840981900000003</v>
-      </c>
-      <c r="ID6">
-        <v>17.649445199999999</v>
+      <c r="IC6" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.486988143594509</v>
+      </c>
+      <c r="ID6" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.739156353282642</v>
       </c>
       <c r="IE6" t="s">
         <v>362</v>
       </c>
       <c r="IF6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IH6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="II6" t="s">
         <v>360</v>
       </c>
       <c r="IJ6" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="IK6" t="s">
         <v>356</v>
@@ -7807,11 +7756,13 @@
       <c r="IL6" t="s">
         <v>356</v>
       </c>
-      <c r="IM6">
-        <v>59.859152799999997</v>
-      </c>
-      <c r="IN6">
-        <v>17.6563135</v>
+      <c r="IM6" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.603545158039779</v>
+      </c>
+      <c r="IN6" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.66998773754883</v>
       </c>
       <c r="IO6" t="s">
         <v>356</v>
@@ -8069,7 +8020,7 @@
         <v>171200693</v>
       </c>
       <c r="LV6" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="LW6">
         <v>4.1080378409999998</v>
@@ -8096,7 +8047,7 @@
         <v>380</v>
       </c>
       <c r="ME6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF6">
         <v>1</v>
@@ -8841,12 +8792,6 @@
       <c r="HZ7" t="s">
         <v>356</v>
       </c>
-      <c r="IA7" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB7" t="s">
-        <v>356</v>
-      </c>
       <c r="IC7" t="s">
         <v>356</v>
       </c>
@@ -9139,7 +9084,7 @@
         <v>171201031</v>
       </c>
       <c r="LV7" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="LW7" t="s">
         <v>356</v>
@@ -9437,12 +9382,6 @@
       <c r="BX8" t="s">
         <v>356</v>
       </c>
-      <c r="BY8" t="s">
-        <v>386</v>
-      </c>
-      <c r="BZ8" t="s">
-        <v>386</v>
-      </c>
       <c r="CA8" t="s">
         <v>356</v>
       </c>
@@ -9453,25 +9392,25 @@
         <v>362</v>
       </c>
       <c r="CD8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="CE8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="CF8" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="CG8" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="CH8" t="s">
-        <v>389</v>
-      </c>
-      <c r="CI8">
-        <v>59.633187100000001</v>
-      </c>
-      <c r="CJ8">
-        <v>16.587987999999999</v>
+        <v>383</v>
+      </c>
+      <c r="CI8" t="s">
+        <v>356</v>
+      </c>
+      <c r="CJ8" t="s">
+        <v>356</v>
       </c>
       <c r="CK8" t="s">
         <v>356</v>
@@ -9911,35 +9850,31 @@
       <c r="HZ8" t="s">
         <v>356</v>
       </c>
-      <c r="IA8" t="s">
-        <v>390</v>
-      </c>
-      <c r="IB8" t="s">
-        <v>390</v>
-      </c>
-      <c r="IC8">
-        <v>59.633187100000001</v>
-      </c>
-      <c r="ID8">
-        <v>16.587987999999999</v>
+      <c r="IC8" s="2">
+        <f t="shared" ref="IC8:IC10" ca="1" si="0">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.090929548696579</v>
+      </c>
+      <c r="ID8" s="2">
+        <f t="shared" ref="ID8:ID10" ca="1" si="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.659656881068386</v>
       </c>
       <c r="IE8" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="IF8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG8" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="IH8" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="II8" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="IJ8" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="IK8" t="s">
         <v>356</v>
@@ -10140,7 +10075,7 @@
         <v>5</v>
       </c>
       <c r="KY8" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="KZ8">
         <v>0</v>
@@ -10209,7 +10144,7 @@
         <v>171201274</v>
       </c>
       <c r="LV8" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="LW8" t="s">
         <v>356</v>
@@ -10224,13 +10159,13 @@
         <v>16</v>
       </c>
       <c r="MA8" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="MB8">
         <v>3</v>
       </c>
       <c r="MC8" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="MD8">
         <v>381</v>
@@ -10251,7 +10186,7 @@
         <v>74972</v>
       </c>
       <c r="MJ8" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="MK8">
         <v>0</v>
@@ -10266,7 +10201,7 @@
         <v>1</v>
       </c>
       <c r="MO8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP8">
         <v>1</v>
@@ -10507,17 +10442,13 @@
       <c r="BX9" t="s">
         <v>356</v>
       </c>
-      <c r="BY9" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ9" t="s">
-        <v>356</v>
-      </c>
-      <c r="CA9">
-        <v>60.254269299999997</v>
-      </c>
-      <c r="CB9">
-        <v>18.373351700000001</v>
+      <c r="CA9" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.050456481755241</v>
+      </c>
+      <c r="CB9" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.381837705895808</v>
       </c>
       <c r="CC9" t="s">
         <v>356</v>
@@ -10537,17 +10468,21 @@
       <c r="CH9" t="s">
         <v>356</v>
       </c>
-      <c r="CI9">
-        <v>59.849038999999998</v>
-      </c>
-      <c r="CJ9">
-        <v>17.679917799999998</v>
-      </c>
-      <c r="CK9">
-        <v>60.254269299999997</v>
-      </c>
-      <c r="CL9">
-        <v>18.373351700000001</v>
+      <c r="CI9" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.400878765384356</v>
+      </c>
+      <c r="CJ9" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.639019922872574</v>
+      </c>
+      <c r="CK9" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.041654185998375</v>
+      </c>
+      <c r="CL9" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.689449167094516</v>
       </c>
       <c r="CM9" t="s">
         <v>356</v>
@@ -10981,35 +10916,31 @@
       <c r="HZ9" t="s">
         <v>356</v>
       </c>
-      <c r="IA9" t="s">
-        <v>399</v>
-      </c>
-      <c r="IB9" t="s">
-        <v>400</v>
-      </c>
-      <c r="IC9">
-        <v>59.849038999999998</v>
-      </c>
-      <c r="ID9">
-        <v>17.679917799999998</v>
+      <c r="IC9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>58.697676430894006</v>
+      </c>
+      <c r="ID9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>17.920649647153443</v>
       </c>
       <c r="IE9" t="s">
         <v>362</v>
       </c>
       <c r="IF9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IH9" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="II9" t="s">
         <v>360</v>
       </c>
       <c r="IJ9" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="IK9" t="s">
         <v>356</v>
@@ -11017,11 +10948,13 @@
       <c r="IL9" t="s">
         <v>356</v>
       </c>
-      <c r="IM9">
-        <v>60.254269299999997</v>
-      </c>
-      <c r="IN9">
-        <v>18.373351700000001</v>
+      <c r="IM9" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.300243751123354</v>
+      </c>
+      <c r="IN9" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.70039770762035</v>
       </c>
       <c r="IO9" t="s">
         <v>356</v>
@@ -11279,7 +11212,7 @@
         <v>171201288</v>
       </c>
       <c r="LV9" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="LW9">
         <v>118.3753439</v>
@@ -11294,19 +11227,19 @@
         <v>16</v>
       </c>
       <c r="MA9" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="MB9">
         <v>3</v>
       </c>
       <c r="MC9" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="MD9">
         <v>382</v>
       </c>
       <c r="ME9" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF9">
         <v>1</v>
@@ -11321,7 +11254,7 @@
         <v>74232</v>
       </c>
       <c r="MJ9" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="MK9">
         <v>0</v>
@@ -11336,7 +11269,7 @@
         <v>1</v>
       </c>
       <c r="MO9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP9">
         <v>1</v>
@@ -11577,17 +11510,13 @@
       <c r="BX10" t="s">
         <v>356</v>
       </c>
-      <c r="BY10" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ10" t="s">
-        <v>356</v>
-      </c>
-      <c r="CA10">
-        <v>59.996917699999997</v>
-      </c>
-      <c r="CB10">
-        <v>17.865814100000001</v>
+      <c r="CA10" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.974309090462654</v>
+      </c>
+      <c r="CB10" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.141846066829878</v>
       </c>
       <c r="CC10" t="s">
         <v>356</v>
@@ -11607,23 +11536,29 @@
       <c r="CH10" t="s">
         <v>356</v>
       </c>
-      <c r="CI10">
-        <v>59.858563799999999</v>
-      </c>
-      <c r="CJ10">
-        <v>17.638926699999999</v>
-      </c>
-      <c r="CK10">
-        <v>59.849566099999997</v>
-      </c>
-      <c r="CL10">
-        <v>17.645247699999999</v>
-      </c>
-      <c r="CM10">
-        <v>59.996917699999997</v>
-      </c>
-      <c r="CN10">
-        <v>17.865814100000001</v>
+      <c r="CI10" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.222229954549825</v>
+      </c>
+      <c r="CJ10" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.021014768259931</v>
+      </c>
+      <c r="CK10" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.338924898117334</v>
+      </c>
+      <c r="CL10" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.086747299202329</v>
+      </c>
+      <c r="CM10" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.065864240253838</v>
+      </c>
+      <c r="CN10" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.893249741577957</v>
       </c>
       <c r="CO10" t="s">
         <v>356</v>
@@ -12051,65 +11986,57 @@
       <c r="HZ10" t="s">
         <v>356</v>
       </c>
-      <c r="IA10" t="s">
-        <v>404</v>
-      </c>
-      <c r="IB10" t="s">
-        <v>404</v>
-      </c>
-      <c r="IC10">
-        <v>59.858563799999999</v>
-      </c>
-      <c r="ID10">
-        <v>17.638926699999999</v>
+      <c r="IC10" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>58.503573707580422</v>
+      </c>
+      <c r="ID10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>17.62558016237762</v>
       </c>
       <c r="IE10" t="s">
         <v>362</v>
       </c>
       <c r="IF10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG10" t="s">
         <v>360</v>
       </c>
       <c r="IH10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="II10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IJ10" t="s">
-        <v>368</v>
-      </c>
-      <c r="IK10" t="s">
-        <v>405</v>
-      </c>
-      <c r="IL10" t="s">
-        <v>406</v>
-      </c>
-      <c r="IM10">
-        <v>59.849566099999997</v>
-      </c>
-      <c r="IN10">
-        <v>17.645247699999999</v>
+        <v>366</v>
+      </c>
+      <c r="IM10" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.623406253652917</v>
+      </c>
+      <c r="IN10" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.352856026521845</v>
       </c>
       <c r="IO10" t="s">
         <v>362</v>
       </c>
       <c r="IP10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IQ10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IR10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="IS10" t="s">
         <v>360</v>
       </c>
       <c r="IT10" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="IU10" t="s">
         <v>356</v>
@@ -12117,11 +12044,13 @@
       <c r="IV10" t="s">
         <v>356</v>
       </c>
-      <c r="IW10">
-        <v>59.996917699999997</v>
-      </c>
-      <c r="IX10">
-        <v>17.865814100000001</v>
+      <c r="IW10" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.58953054961728</v>
+      </c>
+      <c r="IX10" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.830754848440773</v>
       </c>
       <c r="IY10" t="s">
         <v>356</v>
@@ -12280,7 +12209,7 @@
         <v>5</v>
       </c>
       <c r="KY10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="KZ10">
         <v>0</v>
@@ -12349,7 +12278,7 @@
         <v>171201326</v>
       </c>
       <c r="LV10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="LW10">
         <v>41.403596739999998</v>
@@ -12376,7 +12305,7 @@
         <v>380</v>
       </c>
       <c r="ME10" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF10">
         <v>1</v>
@@ -12406,7 +12335,7 @@
         <v>1</v>
       </c>
       <c r="MO10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP10">
         <v>1</v>
@@ -12647,12 +12576,6 @@
       <c r="BX11" t="s">
         <v>356</v>
       </c>
-      <c r="BY11" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ11" t="s">
-        <v>356</v>
-      </c>
       <c r="CA11" t="s">
         <v>356</v>
       </c>
@@ -13121,12 +13044,6 @@
       <c r="HZ11" t="s">
         <v>356</v>
       </c>
-      <c r="IA11" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB11" t="s">
-        <v>356</v>
-      </c>
       <c r="IC11" t="s">
         <v>356</v>
       </c>
@@ -13149,12 +13066,6 @@
         <v>356</v>
       </c>
       <c r="IJ11" t="s">
-        <v>356</v>
-      </c>
-      <c r="IK11" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL11" t="s">
         <v>356</v>
       </c>
       <c r="IM11" t="s">
@@ -13350,7 +13261,7 @@
         <v>2</v>
       </c>
       <c r="KY11" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="KZ11">
         <v>1</v>
@@ -13419,7 +13330,7 @@
         <v>171208182</v>
       </c>
       <c r="LV11" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="LW11" t="s">
         <v>356</v>
@@ -13717,12 +13628,6 @@
       <c r="BX12" t="s">
         <v>356</v>
       </c>
-      <c r="BY12" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ12" t="s">
-        <v>356</v>
-      </c>
       <c r="CA12" t="s">
         <v>356</v>
       </c>
@@ -14191,12 +14096,6 @@
       <c r="HZ12" t="s">
         <v>356</v>
       </c>
-      <c r="IA12" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB12" t="s">
-        <v>356</v>
-      </c>
       <c r="IC12" t="s">
         <v>356</v>
       </c>
@@ -14219,12 +14118,6 @@
         <v>356</v>
       </c>
       <c r="IJ12" t="s">
-        <v>356</v>
-      </c>
-      <c r="IK12" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL12" t="s">
         <v>356</v>
       </c>
       <c r="IM12" t="s">
@@ -14489,7 +14382,7 @@
         <v>171211011</v>
       </c>
       <c r="LV12" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="LW12" t="s">
         <v>356</v>
@@ -14531,7 +14424,7 @@
         <v>75643</v>
       </c>
       <c r="MJ12" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="MK12" t="s">
         <v>360</v>
@@ -14787,17 +14680,13 @@
       <c r="BX13" t="s">
         <v>356</v>
       </c>
-      <c r="BY13" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ13" t="s">
-        <v>356</v>
-      </c>
-      <c r="CA13">
-        <v>59.847388100000003</v>
-      </c>
-      <c r="CB13">
-        <v>17.5962888</v>
+      <c r="CA13" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.733573359330514</v>
+      </c>
+      <c r="CB13" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.054621673870308</v>
       </c>
       <c r="CC13" t="s">
         <v>356</v>
@@ -14817,17 +14706,21 @@
       <c r="CH13" t="s">
         <v>356</v>
       </c>
-      <c r="CI13">
-        <v>59.8580939</v>
-      </c>
-      <c r="CJ13">
-        <v>17.642729299999999</v>
-      </c>
-      <c r="CK13">
-        <v>59.847388100000003</v>
-      </c>
-      <c r="CL13">
-        <v>17.5962888</v>
+      <c r="CI13" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.757696075034126</v>
+      </c>
+      <c r="CJ13" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.717376146929421</v>
+      </c>
+      <c r="CK13" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.684725965659943</v>
+      </c>
+      <c r="CL13" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.572017494170169</v>
       </c>
       <c r="CM13" t="s">
         <v>356</v>
@@ -15261,17 +15154,13 @@
       <c r="HZ13" t="s">
         <v>356</v>
       </c>
-      <c r="IA13" t="s">
-        <v>414</v>
-      </c>
-      <c r="IB13" t="s">
-        <v>356</v>
-      </c>
-      <c r="IC13">
-        <v>59.8580939</v>
-      </c>
-      <c r="ID13">
-        <v>17.642729299999999</v>
+      <c r="IC13" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.053745964067282</v>
+      </c>
+      <c r="ID13" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.070564022862484</v>
       </c>
       <c r="IE13" t="s">
         <v>356</v>
@@ -15291,17 +15180,13 @@
       <c r="IJ13" t="s">
         <v>356</v>
       </c>
-      <c r="IK13" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL13" t="s">
-        <v>356</v>
-      </c>
-      <c r="IM13">
-        <v>59.847388100000003</v>
-      </c>
-      <c r="IN13">
-        <v>17.5962888</v>
+      <c r="IM13" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.431763212854307</v>
+      </c>
+      <c r="IN13" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.318662930648856</v>
       </c>
       <c r="IO13" t="s">
         <v>356</v>
@@ -15559,7 +15444,7 @@
         <v>171214744</v>
       </c>
       <c r="LV13" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="LW13">
         <v>5.7000768239999999</v>
@@ -15586,7 +15471,7 @@
         <v>380</v>
       </c>
       <c r="ME13" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF13">
         <v>1</v>
@@ -15857,12 +15742,6 @@
       <c r="BX14" t="s">
         <v>356</v>
       </c>
-      <c r="BY14" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ14" t="s">
-        <v>356</v>
-      </c>
       <c r="CA14" t="s">
         <v>356</v>
       </c>
@@ -16331,12 +16210,6 @@
       <c r="HZ14" t="s">
         <v>356</v>
       </c>
-      <c r="IA14" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB14" t="s">
-        <v>356</v>
-      </c>
       <c r="IC14" t="s">
         <v>356</v>
       </c>
@@ -16359,12 +16232,6 @@
         <v>356</v>
       </c>
       <c r="IJ14" t="s">
-        <v>356</v>
-      </c>
-      <c r="IK14" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL14" t="s">
         <v>356</v>
       </c>
       <c r="IM14" t="s">
@@ -16629,7 +16496,7 @@
         <v>171216190</v>
       </c>
       <c r="LV14" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="LW14" t="s">
         <v>356</v>
@@ -16644,13 +16511,13 @@
         <v>16</v>
       </c>
       <c r="MA14" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="MB14">
         <v>3</v>
       </c>
       <c r="MC14" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="MD14">
         <v>360</v>
@@ -16671,7 +16538,7 @@
         <v>81576</v>
       </c>
       <c r="MJ14" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="MK14">
         <v>0</v>
@@ -16686,7 +16553,7 @@
         <v>1</v>
       </c>
       <c r="MO14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP14">
         <v>1</v>
@@ -16927,47 +16794,47 @@
       <c r="BX15" t="s">
         <v>356</v>
       </c>
-      <c r="BY15" t="s">
-        <v>418</v>
-      </c>
-      <c r="BZ15" t="s">
-        <v>418</v>
-      </c>
-      <c r="CA15">
-        <v>59.715257000000001</v>
-      </c>
-      <c r="CB15">
-        <v>17.129226200000002</v>
+      <c r="CA15" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.809757522008596</v>
+      </c>
+      <c r="CB15" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.793545533145213</v>
       </c>
       <c r="CC15" t="s">
         <v>362</v>
       </c>
       <c r="CD15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="CE15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="CF15" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="CG15" t="s">
         <v>360</v>
       </c>
       <c r="CH15" t="s">
-        <v>420</v>
-      </c>
-      <c r="CI15">
-        <v>59.715257000000001</v>
-      </c>
-      <c r="CJ15">
-        <v>17.129226200000002</v>
-      </c>
-      <c r="CK15">
-        <v>59.715257000000001</v>
-      </c>
-      <c r="CL15">
-        <v>17.129226200000002</v>
+        <v>406</v>
+      </c>
+      <c r="CI15" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.219805104186378</v>
+      </c>
+      <c r="CJ15" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.517443011496198</v>
+      </c>
+      <c r="CK15" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.855381857351112</v>
+      </c>
+      <c r="CL15" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.30716266842246</v>
       </c>
       <c r="CM15" t="s">
         <v>356</v>
@@ -17401,17 +17268,13 @@
       <c r="HZ15" t="s">
         <v>356</v>
       </c>
-      <c r="IA15" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB15" t="s">
-        <v>356</v>
-      </c>
-      <c r="IC15">
-        <v>59.715257000000001</v>
-      </c>
-      <c r="ID15">
-        <v>17.129226200000002</v>
+      <c r="IC15" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.288804839006708</v>
+      </c>
+      <c r="ID15" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.718378641862259</v>
       </c>
       <c r="IE15" t="s">
         <v>356</v>
@@ -17431,35 +17294,31 @@
       <c r="IJ15" t="s">
         <v>356</v>
       </c>
-      <c r="IK15" t="s">
-        <v>421</v>
-      </c>
-      <c r="IL15" t="s">
-        <v>421</v>
-      </c>
-      <c r="IM15">
-        <v>59.715257000000001</v>
-      </c>
-      <c r="IN15">
-        <v>17.129226200000002</v>
+      <c r="IM15" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.058521570215056</v>
+      </c>
+      <c r="IN15" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.590306746518475</v>
       </c>
       <c r="IO15" t="s">
         <v>362</v>
       </c>
       <c r="IP15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IQ15" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="IR15" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="IS15" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="IT15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IU15" t="s">
         <v>356</v>
@@ -17699,7 +17558,7 @@
         <v>171217280</v>
       </c>
       <c r="LV15" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="LW15" t="s">
         <v>356</v>
@@ -17714,19 +17573,19 @@
         <v>16</v>
       </c>
       <c r="MA15" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="MB15">
         <v>3</v>
       </c>
       <c r="MC15" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="MD15">
         <v>381</v>
       </c>
       <c r="ME15" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF15">
         <v>1</v>
@@ -17741,7 +17600,7 @@
         <v>74596</v>
       </c>
       <c r="MJ15" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="MK15">
         <v>0</v>
@@ -17756,7 +17615,7 @@
         <v>1</v>
       </c>
       <c r="MO15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP15">
         <v>1</v>
@@ -17997,17 +17856,13 @@
       <c r="BX16" t="s">
         <v>356</v>
       </c>
-      <c r="BY16" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ16" t="s">
-        <v>356</v>
-      </c>
-      <c r="CA16">
-        <v>59.9507975</v>
-      </c>
-      <c r="CB16">
-        <v>17.706392600000001</v>
+      <c r="CA16" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.566471918957411</v>
+      </c>
+      <c r="CB16" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.293203778325754</v>
       </c>
       <c r="CC16" t="s">
         <v>356</v>
@@ -18027,17 +17882,21 @@
       <c r="CH16" t="s">
         <v>356</v>
       </c>
-      <c r="CI16">
-        <v>59.862908500000003</v>
-      </c>
-      <c r="CJ16">
-        <v>17.614343000000002</v>
-      </c>
-      <c r="CK16">
-        <v>59.9507975</v>
-      </c>
-      <c r="CL16">
-        <v>17.706392600000001</v>
+      <c r="CI16" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.312649185242648</v>
+      </c>
+      <c r="CJ16" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.952471302254956</v>
+      </c>
+      <c r="CK16" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.618066530814396</v>
+      </c>
+      <c r="CL16" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.368906158383492</v>
       </c>
       <c r="CM16" t="s">
         <v>356</v>
@@ -18471,47 +18330,39 @@
       <c r="HZ16" t="s">
         <v>356</v>
       </c>
-      <c r="IA16" t="s">
-        <v>426</v>
-      </c>
-      <c r="IB16" t="s">
-        <v>426</v>
-      </c>
-      <c r="IC16">
-        <v>59.862908500000003</v>
-      </c>
-      <c r="ID16">
-        <v>17.614343000000002</v>
+      <c r="IC16" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.292238097499748</v>
+      </c>
+      <c r="ID16" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.408159406227249</v>
       </c>
       <c r="IE16" t="s">
         <v>362</v>
       </c>
       <c r="IF16" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG16" t="s">
         <v>360</v>
       </c>
       <c r="IH16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="II16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IJ16" t="s">
-        <v>427</v>
-      </c>
-      <c r="IK16" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL16" t="s">
-        <v>356</v>
-      </c>
-      <c r="IM16">
-        <v>59.9507975</v>
-      </c>
-      <c r="IN16">
-        <v>17.706392600000001</v>
+        <v>411</v>
+      </c>
+      <c r="IM16" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.65705224739488</v>
+      </c>
+      <c r="IN16" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.061878102034857</v>
       </c>
       <c r="IO16" t="s">
         <v>356</v>
@@ -18769,7 +18620,7 @@
         <v>171217337</v>
       </c>
       <c r="LV16" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="LW16">
         <v>22.04910031</v>
@@ -18796,7 +18647,7 @@
         <v>380</v>
       </c>
       <c r="ME16" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF16">
         <v>1</v>
@@ -18811,7 +18662,7 @@
         <v>74340</v>
       </c>
       <c r="MJ16" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="MK16">
         <v>0</v>
@@ -18826,7 +18677,7 @@
         <v>1</v>
       </c>
       <c r="MO16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="MP16">
         <v>1</v>
@@ -19067,12 +18918,6 @@
       <c r="BX17" t="s">
         <v>356</v>
       </c>
-      <c r="BY17" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ17" t="s">
-        <v>356</v>
-      </c>
       <c r="CA17" t="s">
         <v>356</v>
       </c>
@@ -19541,12 +19386,6 @@
       <c r="HZ17" t="s">
         <v>356</v>
       </c>
-      <c r="IA17" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB17" t="s">
-        <v>356</v>
-      </c>
       <c r="IC17" t="s">
         <v>356</v>
       </c>
@@ -19569,12 +19408,6 @@
         <v>356</v>
       </c>
       <c r="IJ17" t="s">
-        <v>356</v>
-      </c>
-      <c r="IK17" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL17" t="s">
         <v>356</v>
       </c>
       <c r="IM17" t="s">
@@ -19839,7 +19672,7 @@
         <v>171220055</v>
       </c>
       <c r="LV17" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="LW17" t="s">
         <v>356</v>
@@ -20137,17 +19970,13 @@
       <c r="BX18" t="s">
         <v>356</v>
       </c>
-      <c r="BY18" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ18" t="s">
-        <v>356</v>
-      </c>
-      <c r="CA18">
-        <v>59.857297799999998</v>
-      </c>
-      <c r="CB18">
-        <v>17.639578499999999</v>
+      <c r="CA18" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.756802020717302</v>
+      </c>
+      <c r="CB18" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.733184266548584</v>
       </c>
       <c r="CC18" t="s">
         <v>356</v>
@@ -20167,18 +19996,16 @@
       <c r="CH18" t="s">
         <v>356</v>
       </c>
-      <c r="CI18">
-        <v>59.857297799999998</v>
-      </c>
-      <c r="CJ18">
-        <v>17.639578499999999</v>
-      </c>
-      <c r="CK18" t="s">
-        <v>356</v>
-      </c>
-      <c r="CL18" t="s">
-        <v>356</v>
-      </c>
+      <c r="CI18" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.582429867012621</v>
+      </c>
+      <c r="CJ18" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.555481884345571</v>
+      </c>
+      <c r="CK18" s="2"/>
+      <c r="CL18" s="2"/>
       <c r="CM18" t="s">
         <v>356</v>
       </c>
@@ -20611,17 +20438,13 @@
       <c r="HZ18" t="s">
         <v>356</v>
       </c>
-      <c r="IA18" t="s">
-        <v>356</v>
-      </c>
-      <c r="IB18" t="s">
-        <v>356</v>
-      </c>
-      <c r="IC18">
-        <v>59.857297799999998</v>
-      </c>
-      <c r="ID18">
-        <v>17.639578499999999</v>
+      <c r="IC18" s="2">
+        <f t="shared" ref="IC18:IC20" ca="1" si="2">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.79627999332363</v>
+      </c>
+      <c r="ID18" s="2">
+        <f t="shared" ref="ID18:ID20" ca="1" si="3">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.987410468937671</v>
       </c>
       <c r="IE18" t="s">
         <v>356</v>
@@ -20639,12 +20462,6 @@
         <v>356</v>
       </c>
       <c r="IJ18" t="s">
-        <v>356</v>
-      </c>
-      <c r="IK18" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL18" t="s">
         <v>356</v>
       </c>
       <c r="IM18" t="s">
@@ -20909,7 +20726,7 @@
         <v>171220793</v>
       </c>
       <c r="LV18" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="LW18" t="s">
         <v>356</v>
@@ -21207,17 +21024,13 @@
       <c r="BX19" t="s">
         <v>356</v>
       </c>
-      <c r="BY19" t="s">
-        <v>356</v>
-      </c>
-      <c r="BZ19" t="s">
-        <v>356</v>
-      </c>
-      <c r="CA19">
-        <v>59.818637799999998</v>
-      </c>
-      <c r="CB19">
-        <v>17.625142799999999</v>
+      <c r="CA19" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.410287270767959</v>
+      </c>
+      <c r="CB19" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.7793417474468</v>
       </c>
       <c r="CC19" t="s">
         <v>356</v>
@@ -21237,17 +21050,21 @@
       <c r="CH19" t="s">
         <v>356</v>
       </c>
-      <c r="CI19">
-        <v>59.881673300000003</v>
-      </c>
-      <c r="CJ19">
-        <v>17.6568051</v>
-      </c>
-      <c r="CK19">
-        <v>59.818637799999998</v>
-      </c>
-      <c r="CL19">
-        <v>17.625142799999999</v>
+      <c r="CI19" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.538987724126969</v>
+      </c>
+      <c r="CJ19" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.313355389007871</v>
+      </c>
+      <c r="CK19" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.150793399634573</v>
+      </c>
+      <c r="CL19" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.889940410672246</v>
       </c>
       <c r="CM19" t="s">
         <v>356</v>
@@ -21681,47 +21498,39 @@
       <c r="HZ19" t="s">
         <v>356</v>
       </c>
-      <c r="IA19" t="s">
-        <v>431</v>
-      </c>
-      <c r="IB19" t="s">
-        <v>432</v>
-      </c>
-      <c r="IC19">
-        <v>59.881673300000003</v>
-      </c>
-      <c r="ID19">
-        <v>17.6568051</v>
+      <c r="IC19" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>58.334759071236512</v>
+      </c>
+      <c r="ID19" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>17.284773250587744</v>
       </c>
       <c r="IE19" t="s">
         <v>362</v>
       </c>
       <c r="IF19" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IH19" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="II19" t="s">
         <v>360</v>
       </c>
       <c r="IJ19" t="s">
-        <v>434</v>
-      </c>
-      <c r="IK19" t="s">
-        <v>356</v>
-      </c>
-      <c r="IL19" t="s">
-        <v>356</v>
-      </c>
-      <c r="IM19">
-        <v>59.818637799999998</v>
-      </c>
-      <c r="IN19">
-        <v>17.625142799999999</v>
+        <v>416</v>
+      </c>
+      <c r="IM19" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.355028470945129</v>
+      </c>
+      <c r="IN19" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.438256239330013</v>
       </c>
       <c r="IO19" t="s">
         <v>356</v>
@@ -21979,7 +21788,7 @@
         <v>171221304</v>
       </c>
       <c r="LV19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="LW19">
         <v>14.43953518</v>
@@ -22006,7 +21815,7 @@
         <v>380</v>
       </c>
       <c r="ME19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="MF19">
         <v>1</v>
@@ -22277,47 +22086,47 @@
       <c r="BX20" t="s">
         <v>356</v>
       </c>
-      <c r="BY20" t="s">
-        <v>435</v>
-      </c>
-      <c r="BZ20" t="s">
-        <v>435</v>
-      </c>
-      <c r="CA20">
-        <v>59.862567300000002</v>
-      </c>
-      <c r="CB20">
-        <v>17.651342</v>
+      <c r="CA20" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.343340384134983</v>
+      </c>
+      <c r="CB20" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.532346350665119</v>
       </c>
       <c r="CC20" t="s">
         <v>362</v>
       </c>
       <c r="CD20" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="CE20" t="s">
         <v>360</v>
       </c>
       <c r="CF20" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="CG20" t="s">
         <v>360</v>
       </c>
       <c r="CH20" t="s">
-        <v>384</v>
-      </c>
-      <c r="CI20">
-        <v>59.850900500000002</v>
-      </c>
-      <c r="CJ20">
-        <v>17.630009300000001</v>
-      </c>
-      <c r="CK20">
-        <v>59.862567300000002</v>
-      </c>
-      <c r="CL20">
-        <v>17.651342</v>
+        <v>379</v>
+      </c>
+      <c r="CI20" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.631063968133255</v>
+      </c>
+      <c r="CJ20" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.100128864431209</v>
+      </c>
+      <c r="CK20" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.491242225036622</v>
+      </c>
+      <c r="CL20" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.118752237228797</v>
       </c>
       <c r="CM20" t="s">
         <v>356</v>
@@ -22751,65 +22560,57 @@
       <c r="HZ20" t="s">
         <v>356</v>
       </c>
-      <c r="IA20" t="s">
-        <v>437</v>
-      </c>
-      <c r="IB20" t="s">
-        <v>438</v>
-      </c>
-      <c r="IC20">
-        <v>59.850900500000002</v>
-      </c>
-      <c r="ID20">
-        <v>17.630009300000001</v>
+      <c r="IC20" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>58.15446311601206</v>
+      </c>
+      <c r="ID20" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>17.429034324195648</v>
       </c>
       <c r="IE20" t="s">
         <v>362</v>
       </c>
       <c r="IF20" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IG20" t="s">
         <v>360</v>
       </c>
       <c r="IH20" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="II20" t="s">
         <v>360</v>
       </c>
       <c r="IJ20" t="s">
-        <v>440</v>
-      </c>
-      <c r="IK20" t="s">
-        <v>441</v>
-      </c>
-      <c r="IL20" t="s">
-        <v>442</v>
-      </c>
-      <c r="IM20">
-        <v>59.862567300000002</v>
-      </c>
-      <c r="IN20">
-        <v>17.651342</v>
+        <v>419</v>
+      </c>
+      <c r="IM20" s="2">
+        <f ca="1">RANDBETWEEN(58,58)+RAND()</f>
+        <v>58.301030849756287</v>
+      </c>
+      <c r="IN20" s="2">
+        <f ca="1">RANDBETWEEN(17,17)+RAND()</f>
+        <v>17.521004063207059</v>
       </c>
       <c r="IO20" t="s">
         <v>362</v>
       </c>
       <c r="IP20" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="IQ20" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="IR20" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="IS20" t="s">
         <v>360</v>
       </c>
       <c r="IT20" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="IU20" t="s">
         <v>356</v>
@@ -23049,7 +22850,7 @@
         <v>180100005</v>
       </c>
       <c r="LV20" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="LW20">
         <v>3.517997228</v>
@@ -23117,8 +22918,16 @@
       <c r="MR20">
         <v>9</v>
       </c>
+    </row>
+    <row r="23" spans="1:356" x14ac:dyDescent="0.25">
+      <c r="CA23" s="2"/>
+      <c r="CC23" s="2"/>
+    </row>
+    <row r="24" spans="1:356" x14ac:dyDescent="0.25">
+      <c r="CA24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>